<commit_message>
[update] 作業報告書 2022/06/29, 30分追記。
</commit_message>
<xml_diff>
--- a/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
+++ b/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>プロジェクト名</t>
     <rPh sb="6" eb="7">
@@ -355,6 +355,14 @@
     <rPh sb="13" eb="15">
       <t>チョウサ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>改修内容・工数調査。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>改修内容・工数調査。</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -649,7 +657,21 @@
     <cellStyle name="桁区切り 2" xfId="5"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1393,7 +1415,7 @@
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C62" sqref="C62:I63"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1465,7 +1487,7 @@
       </c>
       <c r="G8" s="15">
         <f>SUM(G11:G29)</f>
-        <v>73.5</v>
+        <v>85.5</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>5</v>
@@ -1686,21 +1708,37 @@
       <c r="B21" s="18">
         <v>11</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="21"/>
+      <c r="C21" s="19">
+        <v>44741</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="F21" s="22"/>
-      <c r="G21" s="20"/>
+      <c r="G21" s="20">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="18">
         <v>12</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="21"/>
+      <c r="C22" s="19">
+        <v>44742</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>32</v>
+      </c>
       <c r="F22" s="22"/>
-      <c r="G22" s="20"/>
+      <c r="G22" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="18">
@@ -1845,76 +1883,86 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D14:D17 D19">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:C11 C13:C17 B12:B36 C19">
+    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
     <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:C11 C13:C17 B12:B36 C19">
-    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
+  <conditionalFormatting sqref="D23:D28">
     <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+  <conditionalFormatting sqref="C21:C27">
     <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D28">
+  <conditionalFormatting sqref="C12">
     <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C27">
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="D29:D36">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="C29:C36">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29:D36">
+  <conditionalFormatting sqref="C28">
     <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:C36">
+  <conditionalFormatting sqref="D13">
     <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
+  <conditionalFormatting sqref="D18">
     <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
+  <conditionalFormatting sqref="C18">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
+  <conditionalFormatting sqref="D20">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="D21">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
+  <conditionalFormatting sqref="D22">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
@@ -1929,15 +1977,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100E3652DB590BAC84DB2E0D4E8A3DCA88E" ma:contentTypeVersion="12" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="db050205d3e5bcbf08d2a2c60a399ab0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3aa6ddf9-567b-4810-a401-3ff02eef0833" xmlns:ns3="df5e64f4-f615-449d-a6e7-2dd58101ed73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc89e018e03111e1baaf07b6f9284535" ns2:_="" ns3:_="">
     <xsd:import namespace="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
@@ -2156,6 +2195,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2165,14 +2213,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2187,6 +2227,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[update] 作業報告書 2022/09/30 分修正。
</commit_message>
<xml_diff>
--- a/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
+++ b/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
@@ -1077,49 +1077,7 @@
     <cellStyle name="桁区切り 2" xfId="5"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="219">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="213">
     <dxf>
       <fill>
         <patternFill>
@@ -3549,9 +3507,9 @@
   <dimension ref="B1:I68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C62" sqref="C62:I63"/>
-      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4323,7 +4281,7 @@
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="20">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -4513,17 +4471,17 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="218" priority="168" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="168" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11 C15 B12:B68">
-    <cfRule type="expression" dxfId="217" priority="167" stopIfTrue="1">
+    <cfRule type="expression" dxfId="211" priority="167" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="216" priority="166" stopIfTrue="1">
+    <cfRule type="expression" dxfId="210" priority="166" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5058,32 +5016,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5992,492 +5950,492 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D14:D17 D19">
-    <cfRule type="expression" dxfId="103" priority="146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="146" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11 C13:C17 C19 B12:B68">
-    <cfRule type="expression" dxfId="102" priority="145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="145" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="101" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="144" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="100" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="142" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="99" priority="141" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="141" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C27">
-    <cfRule type="expression" dxfId="98" priority="139" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="139" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="97" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="138" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="96" priority="133" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="133" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="95" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="132" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="94" priority="131" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="131" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="93" priority="130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="130" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="92" priority="129" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="129" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="91" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="128" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="90" priority="127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="127" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="89" priority="126" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="126" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="88" priority="125" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="125" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="87" priority="124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="124" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="86" priority="123" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="123" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="85" priority="122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="122" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="84" priority="121" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="121" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="83" priority="120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="120" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="82" priority="119" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="119" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="81" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="118" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="80" priority="117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="117" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="79" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="116" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="78" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="115" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="77" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="114" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="76" priority="113" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="113" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="75" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="112" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="74" priority="111" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="111" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="73" priority="110" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="110" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="72" priority="109" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="109" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="71" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="108" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="70" priority="107" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="107" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="69" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="106" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="68" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="105" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="67" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="88" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="66" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="87" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="65" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="85" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="64" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="84" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="63" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="82" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="62" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="81" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="61" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="79" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="60" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="78" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="59" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="76" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="58" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="75" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="57" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="73" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="56" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="72" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="55" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="70" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="54" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="69" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="53" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="67" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="52" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="66" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="51" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="64" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="50" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="63" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="49" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="61" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="48" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="60" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="47" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="58" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="46" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="57" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="45" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="55" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="44" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="54" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="43" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="52" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="42" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="51" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="41" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="49" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="40" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="48" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="39" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="46" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="38" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="45" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="37" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="43" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="36" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="42" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="35" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="40" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="34" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="39" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="33" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="37" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="32" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="36" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="31" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="34" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="30" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="31" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="30" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="28" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="27" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="25" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="24" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="23" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="22" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="22" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="21" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="21" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="19" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="expression" dxfId="20" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="19" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66">
-    <cfRule type="expression" dxfId="18" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="17" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="16" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="15" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="14" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="13" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:C41">
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:D41">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6491,23 +6449,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100E3652DB590BAC84DB2E0D4E8A3DCA88E" ma:contentTypeVersion="12" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="db050205d3e5bcbf08d2a2c60a399ab0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3aa6ddf9-567b-4810-a401-3ff02eef0833" xmlns:ns3="df5e64f4-f615-449d-a6e7-2dd58101ed73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc89e018e03111e1baaf07b6f9284535" ns2:_="" ns3:_="">
     <xsd:import namespace="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
@@ -6726,10 +6667,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
+    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6752,20 +6721,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
-    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[update] 作業報告書 2022/10/03 分追記。
</commit_message>
<xml_diff>
--- a/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
+++ b/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
   <si>
     <t>プロジェクト名</t>
     <rPh sb="6" eb="7">
@@ -782,6 +782,16 @@
     </rPh>
     <rPh sb="9" eb="11">
       <t>チョウサ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>① 円弧配列 処理フロー作成。</t>
+    <rPh sb="7" eb="9">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>サクセイ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -1077,7 +1087,21 @@
     <cellStyle name="桁区切り 2" xfId="5"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="213">
+  <dxfs count="215">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3509,7 +3533,7 @@
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C62" sqref="C62:I63"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4288,11 +4312,19 @@
       <c r="B48" s="18">
         <v>38</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="21"/>
+      <c r="C48" s="19">
+        <v>44837</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>63</v>
+      </c>
       <c r="F48" s="22"/>
-      <c r="G48" s="20"/>
+      <c r="G48" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="49" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="18">
@@ -4471,577 +4503,577 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D15">
+    <cfRule type="expression" dxfId="214" priority="170" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:C11 C15 B12:B68">
+    <cfRule type="expression" dxfId="213" priority="169" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
     <cfRule type="expression" dxfId="212" priority="168" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:C11 C15 B12:B68">
-    <cfRule type="expression" dxfId="211" priority="167" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="210" priority="166" stopIfTrue="1">
+  <conditionalFormatting sqref="C49">
+    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
+    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="175" priority="86" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule type="expression" dxfId="174" priority="85" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" dxfId="173" priority="84" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule type="expression" dxfId="172" priority="83" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" dxfId="171" priority="82" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="expression" dxfId="170" priority="81" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="175" priority="86" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="expression" dxfId="174" priority="85" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="173" priority="84" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="expression" dxfId="172" priority="83" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="171" priority="82" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="170" priority="81" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="169" priority="80" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="168" priority="79" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="99" priority="2" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="98" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5950,492 +5982,492 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D14:D17 D19">
-    <cfRule type="expression" dxfId="97" priority="146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="146" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11 C13:C17 C19 B12:B68">
-    <cfRule type="expression" dxfId="96" priority="145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="145" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="95" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="144" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="94" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="142" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="93" priority="141" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="141" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C27">
-    <cfRule type="expression" dxfId="92" priority="139" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="139" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="91" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="138" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="90" priority="133" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="133" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="89" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="132" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="88" priority="131" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="131" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="87" priority="130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="130" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="86" priority="129" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="129" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="85" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="128" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="84" priority="127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="127" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="83" priority="126" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="126" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="82" priority="125" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="125" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="81" priority="124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="124" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="80" priority="123" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="123" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="79" priority="122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="122" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="78" priority="121" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="121" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="77" priority="120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="120" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="76" priority="119" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="119" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="75" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="118" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="74" priority="117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="117" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="73" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="116" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="72" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="115" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="71" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="114" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="70" priority="113" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="113" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="69" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="112" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="68" priority="111" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="111" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="67" priority="110" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="110" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="66" priority="109" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="109" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="65" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="108" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="64" priority="107" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="107" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="63" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="106" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="62" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="105" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="61" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="88" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="60" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="87" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="59" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="85" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="58" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="84" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="57" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="82" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="56" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="81" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="55" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="79" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="54" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="78" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="53" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="76" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="52" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="75" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="51" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="73" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="50" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="72" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="49" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="70" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="48" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="69" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="47" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="67" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="46" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="66" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="45" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="64" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="44" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="63" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="43" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="61" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="42" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="60" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="41" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="58" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="40" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="57" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="39" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="55" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="38" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="54" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="37" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="52" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="36" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="51" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="35" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="49" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="34" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="48" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="33" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="46" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="32" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="45" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="31" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="43" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="30" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="42" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="29" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="40" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="28" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="39" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="27" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="37" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="26" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="36" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="25" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="34" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="33" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="23" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="31" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="22" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="30" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="21" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="28" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="20" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="19" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="25" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="18" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="17" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="16" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="15" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66">
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="9" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="6" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="5" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:C41">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:D41">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6449,6 +6481,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100E3652DB590BAC84DB2E0D4E8A3DCA88E" ma:contentTypeVersion="12" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="db050205d3e5bcbf08d2a2c60a399ab0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3aa6ddf9-567b-4810-a401-3ff02eef0833" xmlns:ns3="df5e64f4-f615-449d-a6e7-2dd58101ed73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc89e018e03111e1baaf07b6f9284535" ns2:_="" ns3:_="">
     <xsd:import namespace="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
@@ -6667,14 +6707,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6685,6 +6717,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{792631E2-B910-4E6C-8FB0-3F8857016DB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6703,23 +6752,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{792631E2-B910-4E6C-8FB0-3F8857016DB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
[update] 作業報告書 2022/10/04 分追記。
</commit_message>
<xml_diff>
--- a/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
+++ b/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="65">
   <si>
     <t>プロジェクト名</t>
     <rPh sb="6" eb="7">
@@ -792,6 +792,16 @@
     </rPh>
     <rPh sb="12" eb="14">
       <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>① 円弧配列 テストケース洗い出し。</t>
+    <rPh sb="13" eb="14">
+      <t>アラ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ダ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -3533,7 +3543,7 @@
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C62" sqref="C62:I63"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4330,11 +4340,19 @@
       <c r="B49" s="18">
         <v>39</v>
       </c>
-      <c r="C49" s="19"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="21"/>
+      <c r="C49" s="19">
+        <v>44838</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="F49" s="22"/>
-      <c r="G49" s="20"/>
+      <c r="G49" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="50" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="18">
@@ -4503,576 +4521,576 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="214" priority="170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="172" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11 C15 B12:B68">
-    <cfRule type="expression" dxfId="213" priority="169" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="171" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="212" priority="168" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="170" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
+    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" dxfId="175" priority="86" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule type="expression" dxfId="174" priority="85" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" dxfId="173" priority="84" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="expression" dxfId="172" priority="83" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="175" priority="86" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="expression" dxfId="174" priority="85" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="173" priority="84" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="172" priority="83" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="171" priority="82" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="170" priority="81" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
@@ -6481,11 +6499,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6708,27 +6727,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{792631E2-B910-4E6C-8FB0-3F8857016DB4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6753,9 +6762,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{792631E2-B910-4E6C-8FB0-3F8857016DB4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[update] 作業報告書 2022/10/05 分追記。
</commit_message>
<xml_diff>
--- a/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
+++ b/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
   <si>
     <t>プロジェクト名</t>
     <rPh sb="6" eb="7">
@@ -803,6 +803,10 @@
     <rPh sb="15" eb="16">
       <t>ダ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>① 円弧配列 処理フロー作成。</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3543,7 +3547,7 @@
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C62" sqref="C62:I63"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4358,11 +4362,19 @@
       <c r="B50" s="18">
         <v>40</v>
       </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="21"/>
+      <c r="C50" s="19">
+        <v>44839</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="F50" s="22"/>
-      <c r="G50" s="20"/>
+      <c r="G50" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="51" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="18">
@@ -4521,576 +4533,576 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="214" priority="172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="174" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11 C15 B12:B68">
-    <cfRule type="expression" dxfId="213" priority="171" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="173" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="212" priority="170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="172" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
+    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" dxfId="175" priority="86" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="expression" dxfId="174" priority="85" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="173" priority="76" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="172" priority="75" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49">
+    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="175" priority="86" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="174" priority="85" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="173" priority="84" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="172" priority="83" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
@@ -6499,12 +6511,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6727,17 +6738,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{792631E2-B910-4E6C-8FB0-3F8857016DB4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6762,18 +6783,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{792631E2-B910-4E6C-8FB0-3F8857016DB4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[update] 作業報告書 2022/10/06 分追記。
</commit_message>
<xml_diff>
--- a/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
+++ b/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="66">
   <si>
     <t>プロジェクト名</t>
     <rPh sb="6" eb="7">
@@ -3545,9 +3545,9 @@
   <dimension ref="B1:I68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C62" sqref="C62:I63"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4380,11 +4380,19 @@
       <c r="B51" s="18">
         <v>41</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="21"/>
+      <c r="C51" s="19">
+        <v>44840</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="F51" s="22"/>
-      <c r="G51" s="20"/>
+      <c r="G51" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="52" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="18">
@@ -4533,576 +4541,576 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="214" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="176" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11 C15 B12:B68">
-    <cfRule type="expression" dxfId="213" priority="173" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="175" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="212" priority="172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="174" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
+    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="175" priority="78" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="174" priority="77" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="173" priority="76" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="172" priority="75" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49">
+    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="175" priority="86" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="174" priority="85" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="173" priority="76" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="172" priority="75" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
@@ -6511,14 +6519,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100E3652DB590BAC84DB2E0D4E8A3DCA88E" ma:contentTypeVersion="12" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="db050205d3e5bcbf08d2a2c60a399ab0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3aa6ddf9-567b-4810-a401-3ff02eef0833" xmlns:ns3="df5e64f4-f615-449d-a6e7-2dd58101ed73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc89e018e03111e1baaf07b6f9284535" ns2:_="" ns3:_="">
     <xsd:import namespace="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
@@ -6737,6 +6737,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6747,23 +6755,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{792631E2-B910-4E6C-8FB0-3F8857016DB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6782,6 +6773,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{792631E2-B910-4E6C-8FB0-3F8857016DB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
[update] 作業報告書 2022/10/07 分追記。
</commit_message>
<xml_diff>
--- a/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
+++ b/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
   <si>
     <t>プロジェクト名</t>
     <rPh sb="6" eb="7">
@@ -3547,7 +3547,7 @@
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C62" sqref="C62:I63"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4398,11 +4398,19 @@
       <c r="B52" s="18">
         <v>42</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="21"/>
+      <c r="C52" s="19">
+        <v>44841</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="F52" s="22"/>
-      <c r="G52" s="20"/>
+      <c r="G52" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="53" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="18">
@@ -4541,576 +4549,576 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="214" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="178" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11 C15 B12:B68">
-    <cfRule type="expression" dxfId="213" priority="175" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="177" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="212" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="176" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
+    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="177" priority="80" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="176" priority="79" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="175" priority="78" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="174" priority="77" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="173" priority="76" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="172" priority="75" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49">
+    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="177" priority="88" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="176" priority="87" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="175" priority="78" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="174" priority="77" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="173" priority="76" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="172" priority="75" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
@@ -6519,6 +6527,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100E3652DB590BAC84DB2E0D4E8A3DCA88E" ma:contentTypeVersion="12" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="db050205d3e5bcbf08d2a2c60a399ab0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3aa6ddf9-567b-4810-a401-3ff02eef0833" xmlns:ns3="df5e64f4-f615-449d-a6e7-2dd58101ed73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc89e018e03111e1baaf07b6f9284535" ns2:_="" ns3:_="">
     <xsd:import namespace="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
@@ -6737,38 +6762,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
-    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6791,9 +6788,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
+    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[update] 作業報告書 2022/10/11 分追記。
</commit_message>
<xml_diff>
--- a/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
+++ b/作業報告書/AdvanceCAD⇒AutoCAD移行開発（要件定義）_作業報告書_平.xlsx
@@ -54,7 +54,7 @@
     <definedName name="BD" localSheetId="0">#REF!</definedName>
     <definedName name="BD">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'作業報告書（6～7月）'!$A$1:$H$41</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'作業報告書（8月～）'!$A$1:$H$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'作業報告書（8月～）'!$A$1:$H$71</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'作業報告書（6～7月）'!$9:$10</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'作業報告書（8月～）'!$9:$10</definedName>
     <definedName name="SC_ADDRESS" localSheetId="0">#REF!</definedName>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>プロジェクト名</t>
     <rPh sb="6" eb="7">
@@ -3545,9 +3545,9 @@
   <dimension ref="B1:I68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C62" sqref="C62:I63"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4416,11 +4416,19 @@
       <c r="B53" s="18">
         <v>43</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="21"/>
+      <c r="C53" s="19">
+        <v>44845</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="F53" s="22"/>
-      <c r="G53" s="20"/>
+      <c r="G53" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="54" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="18">
@@ -4443,7 +4451,9 @@
       <c r="G55" s="20"/>
     </row>
     <row r="56" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B56" s="18"/>
+      <c r="B56" s="18">
+        <v>46</v>
+      </c>
       <c r="C56" s="19"/>
       <c r="D56" s="18"/>
       <c r="E56" s="21"/>
@@ -4451,7 +4461,9 @@
       <c r="G56" s="20"/>
     </row>
     <row r="57" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B57" s="18"/>
+      <c r="B57" s="18">
+        <v>47</v>
+      </c>
       <c r="C57" s="19"/>
       <c r="D57" s="18"/>
       <c r="E57" s="21"/>
@@ -4459,7 +4471,9 @@
       <c r="G57" s="20"/>
     </row>
     <row r="58" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B58" s="18"/>
+      <c r="B58" s="18">
+        <v>48</v>
+      </c>
       <c r="C58" s="19"/>
       <c r="D58" s="18"/>
       <c r="E58" s="21"/>
@@ -4467,7 +4481,9 @@
       <c r="G58" s="20"/>
     </row>
     <row r="59" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B59" s="18"/>
+      <c r="B59" s="18">
+        <v>49</v>
+      </c>
       <c r="C59" s="19"/>
       <c r="D59" s="18"/>
       <c r="E59" s="21"/>
@@ -4475,7 +4491,9 @@
       <c r="G59" s="20"/>
     </row>
     <row r="60" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B60" s="18"/>
+      <c r="B60" s="18">
+        <v>50</v>
+      </c>
       <c r="C60" s="19"/>
       <c r="D60" s="18"/>
       <c r="E60" s="21"/>
@@ -4483,7 +4501,9 @@
       <c r="G60" s="20"/>
     </row>
     <row r="61" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B61" s="18"/>
+      <c r="B61" s="18">
+        <v>51</v>
+      </c>
       <c r="C61" s="19"/>
       <c r="D61" s="18"/>
       <c r="E61" s="21"/>
@@ -4491,7 +4511,9 @@
       <c r="G61" s="20"/>
     </row>
     <row r="62" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B62" s="18"/>
+      <c r="B62" s="18">
+        <v>52</v>
+      </c>
       <c r="C62" s="19"/>
       <c r="D62" s="18"/>
       <c r="E62" s="21"/>
@@ -4499,7 +4521,9 @@
       <c r="G62" s="20"/>
     </row>
     <row r="63" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B63" s="18"/>
+      <c r="B63" s="18">
+        <v>53</v>
+      </c>
       <c r="C63" s="19"/>
       <c r="D63" s="18"/>
       <c r="E63" s="21"/>
@@ -4507,7 +4531,9 @@
       <c r="G63" s="20"/>
     </row>
     <row r="64" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B64" s="18"/>
+      <c r="B64" s="18">
+        <v>54</v>
+      </c>
       <c r="C64" s="19"/>
       <c r="D64" s="18"/>
       <c r="E64" s="21"/>
@@ -4515,7 +4541,9 @@
       <c r="G64" s="20"/>
     </row>
     <row r="65" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B65" s="18"/>
+      <c r="B65" s="18">
+        <v>55</v>
+      </c>
       <c r="C65" s="19"/>
       <c r="D65" s="18"/>
       <c r="E65" s="21"/>
@@ -4523,7 +4551,9 @@
       <c r="G65" s="20"/>
     </row>
     <row r="66" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B66" s="18"/>
+      <c r="B66" s="18">
+        <v>56</v>
+      </c>
       <c r="C66" s="19"/>
       <c r="D66" s="18"/>
       <c r="E66" s="21"/>
@@ -4531,7 +4561,9 @@
       <c r="G66" s="20"/>
     </row>
     <row r="67" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B67" s="18"/>
+      <c r="B67" s="18">
+        <v>57</v>
+      </c>
       <c r="C67" s="19"/>
       <c r="D67" s="18"/>
       <c r="E67" s="21"/>
@@ -4539,7 +4571,9 @@
       <c r="G67" s="20"/>
     </row>
     <row r="68" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B68" s="18"/>
+      <c r="B68" s="18">
+        <v>58</v>
+      </c>
       <c r="C68" s="19"/>
       <c r="D68" s="18"/>
       <c r="E68" s="21"/>
@@ -4549,576 +4583,576 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="214" priority="178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="180" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11 C15 B12:B68">
-    <cfRule type="expression" dxfId="213" priority="177" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="179" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="212" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="178" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
+    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="179" priority="82" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="178" priority="81" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="177" priority="80" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="176" priority="79" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="175" priority="78" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="174" priority="77" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="173" priority="76" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="172" priority="75" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49">
+    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="209" priority="120" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="208" priority="119" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="207" priority="118" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="206" priority="117" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="205" priority="116" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="204" priority="115" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="203" priority="114" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="202" priority="113" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="201" priority="112" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="200" priority="111" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="199" priority="110" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="198" priority="109" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="197" priority="108" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="196" priority="107" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="195" priority="106" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="194" priority="105" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="193" priority="104" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="192" priority="103" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="191" priority="102" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="190" priority="101" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="189" priority="100" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="188" priority="99" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="187" priority="98" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="186" priority="97" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="185" priority="96" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="expression" dxfId="184" priority="95" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="183" priority="94" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="expression" dxfId="182" priority="93" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="181" priority="92" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="180" priority="91" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="179" priority="90" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="178" priority="89" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="177" priority="80" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="176" priority="79" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="175" priority="78" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="174" priority="77" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="173" priority="76" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="172" priority="75" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="171" priority="74" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="170" priority="73" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="169" priority="72" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="166" priority="69" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="165" priority="68" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="164" priority="67" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="162" priority="65" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="160" priority="63" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="158" priority="61" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="157" priority="60" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="156" priority="59" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="155" priority="58" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="154" priority="57" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="153" priority="56" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="152" priority="55" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="151" priority="54" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="150" priority="53" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="148" priority="51" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="147" priority="50" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="146" priority="49" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="145" priority="48" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="144" priority="47" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="143" priority="46" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="142" priority="45" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="141" priority="44" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="139" priority="42" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="138" priority="41" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="137" priority="40" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="136" priority="39" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="134" priority="37" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="133" priority="36" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="132" priority="35" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="131" priority="34" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="130" priority="33" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="129" priority="32" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="128" priority="31" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="127" priority="30" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="125" priority="28" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="122" priority="25" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="121" priority="24" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="120" priority="23" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="119" priority="22" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="118" priority="21" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="117" priority="20" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="116" priority="19" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="115" priority="18" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="112" priority="15" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="111" priority="14" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="110" priority="13" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="106" priority="9" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="105" priority="8" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="104" priority="7" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="102" priority="5" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!="済み","TRUE","FALSE")</formula>
     </cfRule>
@@ -6527,23 +6561,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100E3652DB590BAC84DB2E0D4E8A3DCA88E" ma:contentTypeVersion="12" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="db050205d3e5bcbf08d2a2c60a399ab0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3aa6ddf9-567b-4810-a401-3ff02eef0833" xmlns:ns3="df5e64f4-f615-449d-a6e7-2dd58101ed73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc89e018e03111e1baaf07b6f9284535" ns2:_="" ns3:_="">
     <xsd:import namespace="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
@@ -6762,10 +6779,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x7c21__x6613__x8aac__x660e_ xmlns="3aa6ddf9-567b-4810-a401-3ff02eef0833" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
+    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6788,20 +6833,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BB3938-5547-4468-9224-E3EA75CBEE7B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3F82381-36CE-4A8E-8346-65B8C1E6764F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3aa6ddf9-567b-4810-a401-3ff02eef0833"/>
-    <ds:schemaRef ds:uri="df5e64f4-f615-449d-a6e7-2dd58101ed73"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>